<commit_message>
alguns problemas da OBI
</commit_message>
<xml_diff>
--- a/spoj_br/Resolvidos.xlsx
+++ b/spoj_br/Resolvidos.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
     <t>ID</t>
   </si>
@@ -43,6 +43,27 @@
   </si>
   <si>
     <t>JBUSCA12</t>
+  </si>
+  <si>
+    <t>Soma</t>
+  </si>
+  <si>
+    <t>função recursiva</t>
+  </si>
+  <si>
+    <t>Fatorial</t>
+  </si>
+  <si>
+    <t>SOMA</t>
+  </si>
+  <si>
+    <t>FATORIA2</t>
+  </si>
+  <si>
+    <t>Quermesse</t>
+  </si>
+  <si>
+    <t>QUERM</t>
   </si>
 </sst>
 </file>
@@ -384,10 +405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -440,6 +461,48 @@
         <v>6</v>
       </c>
     </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3830</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>3774</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>811</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>